<commit_message>
adding matrix to document
</commit_message>
<xml_diff>
--- a/Documents/Budget Document/Parts.xlsx
+++ b/Documents/Budget Document/Parts.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kurt\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24709"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30780" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -153,7 +151,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +193,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -218,12 +231,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -233,8 +249,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -295,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +350,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,7 +527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,459 +535,470 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E6:P35"/>
+  <dimension ref="E6:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:14">
       <c r="F6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+    <row r="7" spans="5:14">
+      <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
+    <row r="8" spans="5:14" ht="16">
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2">
+        <v>40.22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="5:14">
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="2">
-        <v>40.22</v>
+        <v>38.89</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="K9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L9" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="L9">
+        <v>40</v>
       </c>
       <c r="M9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="5:14">
+      <c r="E10" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="4">
+        <v>135</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10">
+        <v>76</v>
+      </c>
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="5:14">
+      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="2">
-        <v>38.89</v>
-      </c>
-      <c r="I10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10">
-        <v>40</v>
-      </c>
-      <c r="M10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="4">
-        <v>135</v>
+      <c r="H11" s="2">
+        <v>65.900000000000006</v>
       </c>
       <c r="I11" t="s">
         <v>28</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L11">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="5:14">
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>5</v>
+      </c>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <v>6</v>
+      </c>
+      <c r="N13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="5:14">
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <v>7</v>
+      </c>
+      <c r="M14">
+        <v>8</v>
+      </c>
+      <c r="N14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="5:14">
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>8</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>9</v>
+      </c>
+      <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="N15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="5:14">
+      <c r="F16" t="s">
         <v>31</v>
       </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="2">
-        <v>65.900000000000006</v>
-      </c>
-      <c r="I12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12">
-        <v>65</v>
-      </c>
-      <c r="M12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <v>7</v>
+      </c>
+      <c r="L16">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>8</v>
+      </c>
+      <c r="N16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="6:16">
+      <c r="H18">
+        <v>0.2</v>
+      </c>
+      <c r="I18">
+        <v>0.2</v>
+      </c>
+      <c r="J18">
+        <v>0.1</v>
+      </c>
+      <c r="K18">
+        <v>0.25</v>
+      </c>
+      <c r="L18">
+        <v>0.1</v>
+      </c>
+      <c r="M18">
+        <v>0.1</v>
+      </c>
+      <c r="N18">
+        <v>0.05</v>
+      </c>
+      <c r="O18">
+        <f>SUM(H18:N18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="6:16">
+      <c r="F20" t="s">
         <v>12</v>
       </c>
-      <c r="H19">
-        <v>8</v>
-      </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
-      </c>
-      <c r="K19">
-        <v>5</v>
-      </c>
-      <c r="L19">
-        <v>8</v>
-      </c>
-      <c r="M19">
-        <v>6</v>
-      </c>
-      <c r="N19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
+      <c r="H20">
+        <f>H13*H18</f>
+        <v>1.6</v>
+      </c>
+      <c r="I20">
+        <f>I13*I18</f>
+        <v>0.4</v>
+      </c>
+      <c r="J20">
+        <f>J13*J18</f>
+        <v>0.2</v>
+      </c>
+      <c r="K20">
+        <f>K13*K18</f>
+        <v>1.25</v>
+      </c>
+      <c r="L20">
+        <f>L13*L18</f>
+        <v>0.8</v>
+      </c>
+      <c r="M20">
+        <f>M13*M18</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="N20">
+        <f>N13*N18</f>
+        <v>0.45</v>
+      </c>
+      <c r="P20">
+        <f>SUM(H20:N20)</f>
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="21" spans="6:16">
+      <c r="F21" t="s">
         <v>17</v>
       </c>
-      <c r="H20">
-        <v>9</v>
-      </c>
-      <c r="I20">
-        <v>5</v>
-      </c>
-      <c r="J20">
-        <v>5</v>
-      </c>
-      <c r="K20">
-        <v>9</v>
-      </c>
-      <c r="L20">
-        <v>7</v>
-      </c>
-      <c r="M20">
-        <v>8</v>
-      </c>
-      <c r="N20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
+      <c r="H21">
+        <f>H14*H18</f>
+        <v>1.8</v>
+      </c>
+      <c r="I21">
+        <f>I14*I18</f>
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <f>J14*J18</f>
+        <v>0.5</v>
+      </c>
+      <c r="K21">
+        <f>K14*K18</f>
+        <v>2.25</v>
+      </c>
+      <c r="L21">
+        <f>L14*L18</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="M21">
+        <f>M14*M18</f>
+        <v>0.8</v>
+      </c>
+      <c r="N21">
+        <f>N14*N18</f>
+        <v>0.45</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ref="P21:P23" si="0">SUM(H21:N21)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="22" spans="6:16">
+      <c r="F22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21">
-        <v>8</v>
-      </c>
-      <c r="J21">
-        <v>8</v>
-      </c>
-      <c r="K21">
-        <v>10</v>
-      </c>
-      <c r="L21">
-        <v>9</v>
-      </c>
-      <c r="M21">
-        <v>10</v>
-      </c>
-      <c r="N21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
+      <c r="G22" s="6"/>
+      <c r="H22" s="6">
+        <f>H15*H18</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="I22" s="6">
+        <f>I15*I18</f>
+        <v>1.6</v>
+      </c>
+      <c r="J22" s="6">
+        <f>J15*J18</f>
+        <v>0.8</v>
+      </c>
+      <c r="K22" s="6">
+        <f>K15*K18</f>
+        <v>2.5</v>
+      </c>
+      <c r="L22" s="6">
+        <f>L15*L18</f>
+        <v>0.9</v>
+      </c>
+      <c r="M22" s="6">
+        <f>M15*M18</f>
+        <v>1</v>
+      </c>
+      <c r="N22" s="6">
+        <f>N15*N18</f>
+        <v>0.25</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6">
+        <f t="shared" si="0"/>
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="23" spans="6:16">
+      <c r="F23" t="s">
         <v>31</v>
       </c>
-      <c r="H22">
-        <v>5</v>
-      </c>
-      <c r="I22">
-        <v>8</v>
-      </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
-      <c r="K22">
-        <v>7</v>
-      </c>
-      <c r="L22">
-        <v>8</v>
-      </c>
-      <c r="M22">
-        <v>8</v>
-      </c>
-      <c r="N22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H30">
-        <v>0.2</v>
-      </c>
-      <c r="I30">
-        <v>0.2</v>
-      </c>
-      <c r="J30">
-        <v>0.1</v>
-      </c>
-      <c r="K30">
-        <v>0.25</v>
-      </c>
-      <c r="L30">
-        <v>0.1</v>
-      </c>
-      <c r="M30">
-        <v>0.1</v>
-      </c>
-      <c r="N30">
-        <v>0.05</v>
-      </c>
-      <c r="O30">
-        <f>SUM(H30:N30)</f>
+      <c r="H23">
+        <f>H16*H18</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32">
-        <f>H19*H30</f>
+      <c r="I23">
+        <f>I16*I18</f>
         <v>1.6</v>
       </c>
-      <c r="I32">
-        <f t="shared" ref="I32:N32" si="0">I19*I30</f>
-        <v>0.4</v>
-      </c>
-      <c r="J32">
+      <c r="J23">
+        <f>J16*J18</f>
+        <v>0.5</v>
+      </c>
+      <c r="K23">
+        <f>K16*K18</f>
+        <v>1.75</v>
+      </c>
+      <c r="L23">
+        <f>L16*L18</f>
+        <v>0.8</v>
+      </c>
+      <c r="M23">
+        <f>M16*M18</f>
+        <v>0.8</v>
+      </c>
+      <c r="N23">
+        <f>N16*N18</f>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="0"/>
-        <v>1.25</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
-      </c>
-      <c r="P32">
-        <f>SUM(H32:N32)</f>
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="33" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33">
-        <f>H20*H30</f>
-        <v>1.8</v>
-      </c>
-      <c r="I33">
-        <f t="shared" ref="I33:N33" si="1">I20*I30</f>
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="1"/>
-        <v>2.25</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="1"/>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="1"/>
-        <v>0.45</v>
-      </c>
-      <c r="P33">
-        <f t="shared" ref="P33:P35" si="2">SUM(H33:N33)</f>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="34" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F34" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6">
-        <f>H21*H30</f>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="I34" s="6">
-        <f t="shared" ref="I34:N34" si="3">I21*I30</f>
-        <v>1.6</v>
-      </c>
-      <c r="J34" s="6">
-        <f t="shared" si="3"/>
-        <v>0.8</v>
-      </c>
-      <c r="K34" s="6">
-        <f t="shared" si="3"/>
-        <v>2.5</v>
-      </c>
-      <c r="L34" s="6">
-        <f t="shared" si="3"/>
-        <v>0.9</v>
-      </c>
-      <c r="M34" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N34" s="6">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6">
-        <f t="shared" si="2"/>
-        <v>7.65</v>
-      </c>
-    </row>
-    <row r="35" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H35">
-        <f>H22*H30</f>
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <f t="shared" ref="I35:N35" si="4">I22*I30</f>
-        <v>1.6</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="4"/>
-        <v>1.75</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="4"/>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="2"/>
         <v>6.7999999999999989</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1" display="http://www.ti.com/product/am3358"/>
+    <hyperlink ref="E11" r:id="rId1" display="http://www.ti.com/product/am3358"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>